<commit_message>
analysis and data results from the previous and update embedding for the answer list
</commit_message>
<xml_diff>
--- a/Result and Analysis Section/Second pass model outputs/t5_small hard grids - with time data.xlsx
+++ b/Result and Analysis Section/Second pass model outputs/t5_small hard grids - with time data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parzi\OneDrive - Tribhuvan University\Desktop\Major Project\CODE\BCS Code\BCS-ALL-Code\Crossword Solver\Result and Analysis Section\Second pass model outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{ED614009-1484-4668-B996-76732FD5B30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82B1C8A-427C-4C99-ABC1-F036638A0156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t5_small hard grids - with time" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -31,9 +31,6 @@
     <t>S_Pass Call Count</t>
   </si>
   <si>
-    <t>First Pass Model</t>
-  </si>
-  <si>
     <t>Second Pass Model
 (T5-Small)</t>
   </si>
@@ -41,21 +38,42 @@
     <t>T5-Small Time Data</t>
   </si>
   <si>
-    <t>Letter Accuracy</t>
+    <t>Second Pass Model
+(ByT5-Small)</t>
   </si>
   <si>
-    <t>Word Accuracy</t>
+    <t>First Pass Model Accuracies</t>
   </si>
   <si>
-    <t>Second Pass Model
-(ByT5-Small)</t>
+    <t>Letter</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Time to Infer
+(per pair) ms</t>
+  </si>
+  <si>
+    <t>Time to Infer 
+(Per Pair)
+ms</t>
+  </si>
+  <si>
+    <t>Accuracies</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>S.N.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,8 +208,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,8 +402,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -487,6 +524,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -532,7 +654,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -540,17 +662,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -906,923 +1064,1129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="J21" sqref="A1:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:20" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="R1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="6" t="s">
+      <c r="S1" s="3"/>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="13"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="R3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
         <v>45127</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="7">
         <v>93.44</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D4" s="7">
         <v>79.489999999999995</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E4" s="7">
         <v>95.63</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F4" s="7">
         <v>83.33</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G4" s="5">
+        <f>(R4/S4) * 1000</f>
+        <v>89.849151313984791</v>
+      </c>
+      <c r="H4" s="7">
+        <v>95.63</v>
+      </c>
+      <c r="I4" s="7">
+        <v>83.33</v>
+      </c>
+      <c r="J4" s="5">
+        <f>(M4/N4) * 1000</f>
+        <v>415.2083365540754</v>
+      </c>
+      <c r="M4" s="2">
+        <v>2335.1316847801199</v>
+      </c>
+      <c r="N4" s="2">
+        <v>5624</v>
+      </c>
+      <c r="O4">
+        <f>(M4/N4) * 1000</f>
+        <v>415.2083365540754</v>
+      </c>
+      <c r="R4" s="2">
         <v>354.45490193366999</v>
       </c>
-      <c r="H3" s="2">
+      <c r="S4" s="2">
         <v>3945</v>
       </c>
-      <c r="I3" s="2">
-        <f>(G3/H3) * 1000</f>
+      <c r="T4" s="2">
+        <f>(R4/S4) * 1000</f>
         <v>89.849151313984791</v>
       </c>
-      <c r="J3" s="2">
-        <v>95.63</v>
-      </c>
-      <c r="K3" s="2">
-        <v>83.33</v>
-      </c>
-      <c r="L3" s="2">
-        <v>2335.1316847801199</v>
-      </c>
-      <c r="M3" s="2">
-        <v>5624</v>
-      </c>
-      <c r="N3">
-        <f>(L3/M3) * 1000</f>
-        <v>415.2083365540754</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3">
+    </row>
+    <row r="5" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10">
         <v>45134</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="8">
         <v>97.84</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="8">
         <v>92.31</v>
       </c>
-      <c r="E4" s="2">
-        <v>100</v>
-      </c>
-      <c r="F4" s="2">
-        <v>100</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="E5" s="8">
+        <v>100</v>
+      </c>
+      <c r="F5" s="8">
+        <v>100</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" ref="G5:G21" si="0">(R5/S5) * 1000</f>
+        <v>6.8626967383443676</v>
+      </c>
+      <c r="H5" s="8">
+        <v>100</v>
+      </c>
+      <c r="I5" s="8">
+        <v>100</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" ref="J5:J21" si="1">(M5/N5) * 1000</f>
+        <v>33.276469511946765</v>
+      </c>
+      <c r="M5" s="2">
+        <v>200.02485823631201</v>
+      </c>
+      <c r="N5" s="2">
+        <v>6011</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ref="O5:O21" si="2">(M5/N5) * 1000</f>
+        <v>33.276469511946765</v>
+      </c>
+      <c r="R5" s="2">
         <v>29.729202270507798</v>
       </c>
-      <c r="H4" s="2">
+      <c r="S5" s="2">
         <v>4332</v>
       </c>
-      <c r="I4" s="2">
-        <f t="shared" ref="I4:I20" si="0">(G4/H4) * 1000</f>
+      <c r="T5" s="2">
+        <f t="shared" ref="T5:T20" si="3">(R5/S5) * 1000</f>
         <v>6.8626967383443676</v>
       </c>
-      <c r="J4" s="2">
-        <v>100</v>
-      </c>
-      <c r="K4" s="2">
-        <v>100</v>
-      </c>
-      <c r="L4" s="2">
-        <v>200.02485823631201</v>
-      </c>
-      <c r="M4" s="2">
-        <v>6011</v>
-      </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N20" si="1">(L4/M4) * 1000</f>
-        <v>33.276469511946765</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
+    </row>
+    <row r="6" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10">
         <v>45151</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="8">
         <v>99.72</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="8">
         <v>98.51</v>
       </c>
-      <c r="E5" s="2">
-        <v>100</v>
-      </c>
-      <c r="F5" s="2">
-        <v>100</v>
-      </c>
-      <c r="G5" s="2">
-        <v>24.735080957412698</v>
-      </c>
-      <c r="H5" s="2">
-        <v>4633</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="E6" s="8">
+        <v>100</v>
+      </c>
+      <c r="F6" s="8">
+        <v>100</v>
+      </c>
+      <c r="G6" s="6">
         <f t="shared" si="0"/>
         <v>5.3388907743174396</v>
       </c>
-      <c r="J5" s="2">
-        <v>100</v>
-      </c>
-      <c r="K5" s="2">
-        <v>100</v>
-      </c>
-      <c r="L5" s="2">
-        <v>158.10435748100201</v>
-      </c>
-      <c r="M5" s="2">
-        <v>6312</v>
-      </c>
-      <c r="N5">
+      <c r="H6" s="8">
+        <v>100</v>
+      </c>
+      <c r="I6" s="8">
+        <v>100</v>
+      </c>
+      <c r="J6" s="6">
         <f t="shared" si="1"/>
         <v>25.048218865811471</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="M6" s="2">
+        <v>158.10435748100201</v>
+      </c>
+      <c r="N6" s="2">
+        <v>6312</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>25.048218865811471</v>
+      </c>
+      <c r="R6" s="2">
+        <v>24.735080957412698</v>
+      </c>
+      <c r="S6" s="2">
+        <v>4633</v>
+      </c>
+      <c r="T6" s="2">
+        <f t="shared" si="3"/>
+        <v>5.3388907743174396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="10">
         <v>45155</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="8">
         <v>97.85</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="8">
         <v>91.03</v>
       </c>
-      <c r="E6" s="2">
-        <v>100</v>
-      </c>
-      <c r="F6" s="2">
-        <v>100</v>
-      </c>
-      <c r="G6" s="2">
-        <v>32.4898035526275</v>
-      </c>
-      <c r="H6" s="2">
-        <v>5039</v>
-      </c>
-      <c r="I6" s="2">
+      <c r="E7" s="8">
+        <v>100</v>
+      </c>
+      <c r="F7" s="8">
+        <v>100</v>
+      </c>
+      <c r="G7" s="6">
         <f t="shared" si="0"/>
         <v>6.4476688931588608</v>
       </c>
-      <c r="J6" s="2">
-        <v>100</v>
-      </c>
-      <c r="K6" s="2">
-        <v>100</v>
-      </c>
-      <c r="L6" s="2">
-        <v>238.00237679481501</v>
-      </c>
-      <c r="M6" s="2">
-        <v>6718</v>
-      </c>
-      <c r="N6">
+      <c r="H7" s="8">
+        <v>100</v>
+      </c>
+      <c r="I7" s="8">
+        <v>100</v>
+      </c>
+      <c r="J7" s="6">
         <f t="shared" si="1"/>
         <v>35.427564274310065</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="M7" s="2">
+        <v>238.00237679481501</v>
+      </c>
+      <c r="N7" s="2">
+        <v>6718</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>35.427564274310065</v>
+      </c>
+      <c r="R7" s="2">
+        <v>32.4898035526275</v>
+      </c>
+      <c r="S7" s="2">
+        <v>5039</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" si="3"/>
+        <v>6.4476688931588608</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
+      <c r="B8" s="10">
         <v>45156</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="8">
         <v>96.3</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="8">
         <v>90.28</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="8">
         <v>97.35</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="8">
         <v>93.06</v>
       </c>
-      <c r="G7" s="2">
-        <v>66.013350963592501</v>
-      </c>
-      <c r="H7" s="2">
-        <v>5743</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="G8" s="6">
         <f t="shared" si="0"/>
         <v>11.494576173357565</v>
       </c>
-      <c r="J7" s="2">
-        <v>100</v>
-      </c>
-      <c r="K7" s="2">
-        <v>100</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1004.0551571846</v>
-      </c>
-      <c r="M7" s="2">
-        <v>8232</v>
-      </c>
-      <c r="N7">
+      <c r="H8" s="8">
+        <v>100</v>
+      </c>
+      <c r="I8" s="8">
+        <v>100</v>
+      </c>
+      <c r="J8" s="6">
         <f t="shared" si="1"/>
         <v>121.96977128092809</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="M8" s="2">
+        <v>1004.0551571846</v>
+      </c>
+      <c r="N8" s="2">
+        <v>8232</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>121.96977128092809</v>
+      </c>
+      <c r="R8" s="2">
+        <v>66.013350963592501</v>
+      </c>
+      <c r="S8" s="2">
+        <v>5743</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="3"/>
+        <v>11.494576173357565</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="10">
         <v>45168</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="8">
         <v>95.7</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="8">
         <v>83.33</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="8">
         <v>98.92</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="8">
         <v>94.87</v>
       </c>
-      <c r="G8" s="2">
-        <v>70.237010717391897</v>
-      </c>
-      <c r="H8" s="2">
-        <v>6543</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="G9" s="6">
         <f t="shared" si="0"/>
         <v>10.734679920127144</v>
       </c>
-      <c r="J8" s="2">
+      <c r="H9" s="8">
         <v>98.92</v>
       </c>
-      <c r="K8" s="2">
+      <c r="I9" s="8">
         <v>94.87</v>
       </c>
-      <c r="L8" s="2">
-        <v>428.64082455635003</v>
-      </c>
-      <c r="M8" s="2">
-        <v>9032</v>
-      </c>
-      <c r="N8">
+      <c r="J9" s="6">
         <f t="shared" si="1"/>
         <v>47.458018662129099</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="M9" s="2">
+        <v>428.64082455635003</v>
+      </c>
+      <c r="N9" s="2">
+        <v>9032</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>47.458018662129099</v>
+      </c>
+      <c r="R9" s="2">
+        <v>70.237010717391897</v>
+      </c>
+      <c r="S9" s="2">
+        <v>6543</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="3"/>
+        <v>10.734679920127144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="10">
         <v>45170</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C10" s="8">
         <v>99.49</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="8">
         <v>97.22</v>
       </c>
-      <c r="E9" s="2">
-        <v>100</v>
-      </c>
-      <c r="F9" s="2">
-        <v>100</v>
-      </c>
-      <c r="G9" s="2">
-        <v>14.051763534545801</v>
-      </c>
-      <c r="H9" s="2">
-        <v>6737</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="E10" s="8">
+        <v>100</v>
+      </c>
+      <c r="F10" s="8">
+        <v>100</v>
+      </c>
+      <c r="G10" s="6">
         <f t="shared" si="0"/>
         <v>2.0857597646646577</v>
       </c>
-      <c r="J9" s="2">
-        <v>100</v>
-      </c>
-      <c r="K9" s="2">
-        <v>100</v>
-      </c>
-      <c r="L9" s="2">
-        <v>98.668484687805105</v>
-      </c>
-      <c r="M9" s="2">
-        <v>9226</v>
-      </c>
-      <c r="N9">
+      <c r="H10" s="8">
+        <v>100</v>
+      </c>
+      <c r="I10" s="8">
+        <v>100</v>
+      </c>
+      <c r="J10" s="6">
         <f t="shared" si="1"/>
         <v>10.694611390397258</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3">
+      <c r="M10" s="2">
+        <v>98.668484687805105</v>
+      </c>
+      <c r="N10" s="2">
+        <v>9226</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>10.694611390397258</v>
+      </c>
+      <c r="R10" s="2">
+        <v>14.051763534545801</v>
+      </c>
+      <c r="S10" s="2">
+        <v>6737</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0857597646646577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
+      <c r="B11" s="10">
         <v>45177</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C11" s="8">
         <v>98.46</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="8">
         <v>91.67</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="8">
         <v>99.49</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="8">
         <v>97.22</v>
       </c>
-      <c r="G10" s="2">
-        <v>53.333485364913898</v>
-      </c>
-      <c r="H10" s="2">
-        <v>7287</v>
-      </c>
-      <c r="I10" s="2">
+      <c r="G11" s="6">
         <f t="shared" si="0"/>
         <v>7.3189907183908192</v>
       </c>
-      <c r="J10" s="2">
+      <c r="H11" s="8">
         <v>99.49</v>
       </c>
-      <c r="K10" s="2">
+      <c r="I11" s="8">
         <v>97.22</v>
       </c>
-      <c r="L10" s="2">
-        <v>274.491716861724</v>
-      </c>
-      <c r="M10" s="2">
-        <v>9776</v>
-      </c>
-      <c r="N10">
+      <c r="J11" s="6">
         <f t="shared" si="1"/>
         <v>28.078121610241816</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3">
+      <c r="M11" s="2">
+        <v>274.491716861724</v>
+      </c>
+      <c r="N11" s="2">
+        <v>9776</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>28.078121610241816</v>
+      </c>
+      <c r="R11" s="2">
+        <v>53.333485364913898</v>
+      </c>
+      <c r="S11" s="2">
+        <v>7287</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="3"/>
+        <v>7.3189907183908192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>9</v>
+      </c>
+      <c r="B12" s="10">
         <v>45184</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C12" s="8">
         <v>97.89</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="8">
         <v>90.32</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="8">
         <v>99.47</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="8">
         <v>96.77</v>
       </c>
-      <c r="G11" s="2">
-        <v>83.321228981017995</v>
-      </c>
-      <c r="H11" s="2">
-        <v>8085</v>
-      </c>
-      <c r="I11" s="2">
+      <c r="G12" s="6">
         <f t="shared" si="0"/>
         <v>10.305656027336795</v>
       </c>
-      <c r="J11" s="2">
-        <v>100</v>
-      </c>
-      <c r="K11" s="2">
-        <v>100</v>
-      </c>
-      <c r="L11" s="2">
-        <v>358.201133728027</v>
-      </c>
-      <c r="M11" s="2">
-        <v>10576</v>
-      </c>
-      <c r="N11">
+      <c r="H12" s="8">
+        <v>100</v>
+      </c>
+      <c r="I12" s="8">
+        <v>100</v>
+      </c>
+      <c r="J12" s="6">
         <f t="shared" si="1"/>
         <v>33.869244868383795</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3">
+      <c r="M12" s="2">
+        <v>358.201133728027</v>
+      </c>
+      <c r="N12" s="2">
+        <v>10576</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>33.869244868383795</v>
+      </c>
+      <c r="R12" s="2">
+        <v>83.321228981017995</v>
+      </c>
+      <c r="S12" s="2">
+        <v>8085</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="3"/>
+        <v>10.305656027336795</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>10</v>
+      </c>
+      <c r="B13" s="10">
         <v>45185</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C13" s="8">
         <v>99.48</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="8">
         <v>96.97</v>
       </c>
-      <c r="E12" s="2">
-        <v>100</v>
-      </c>
-      <c r="F12" s="2">
-        <v>100</v>
-      </c>
-      <c r="G12" s="2">
-        <v>11.4732353687286</v>
-      </c>
-      <c r="H12" s="2">
-        <v>8235</v>
-      </c>
-      <c r="I12" s="2">
+      <c r="E13" s="8">
+        <v>100</v>
+      </c>
+      <c r="F13" s="8">
+        <v>100</v>
+      </c>
+      <c r="G13" s="6">
         <f t="shared" si="0"/>
         <v>1.3932283386434245</v>
       </c>
-      <c r="J12" s="2">
-        <v>100</v>
-      </c>
-      <c r="K12" s="2">
-        <v>100</v>
-      </c>
-      <c r="L12" s="2">
-        <v>65.030074834823594</v>
-      </c>
-      <c r="M12" s="2">
-        <v>10726</v>
-      </c>
-      <c r="N12">
+      <c r="H13" s="8">
+        <v>100</v>
+      </c>
+      <c r="I13" s="8">
+        <v>100</v>
+      </c>
+      <c r="J13" s="6">
         <f t="shared" si="1"/>
         <v>6.0628449407816145</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3">
+      <c r="M13" s="2">
+        <v>65.030074834823594</v>
+      </c>
+      <c r="N13" s="2">
+        <v>10726</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>6.0628449407816145</v>
+      </c>
+      <c r="R13" s="2">
+        <v>11.4732353687286</v>
+      </c>
+      <c r="S13" s="2">
+        <v>8235</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="3"/>
+        <v>1.3932283386434245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>11</v>
+      </c>
+      <c r="B14" s="10">
         <v>45203</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C14" s="8">
         <v>95.11</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="8">
         <v>83.33</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="8">
         <v>95.65</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="8">
         <v>84.62</v>
       </c>
-      <c r="G13" s="2">
-        <v>18.381932973861598</v>
-      </c>
-      <c r="H13" s="2">
-        <v>8452</v>
-      </c>
-      <c r="I13" s="2">
+      <c r="G14" s="6">
         <f t="shared" si="0"/>
         <v>2.1748619230787503</v>
       </c>
-      <c r="J13" s="2">
+      <c r="H14" s="8">
         <v>95.65</v>
       </c>
-      <c r="K13" s="2">
+      <c r="I14" s="8">
         <v>84.62</v>
       </c>
-      <c r="L13" s="2">
-        <v>125.76925969123801</v>
-      </c>
-      <c r="M13" s="2">
-        <v>10943</v>
-      </c>
-      <c r="N13">
+      <c r="J14" s="6">
         <f t="shared" si="1"/>
         <v>11.493124343529015</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="M14" s="2">
+        <v>125.76925969123801</v>
+      </c>
+      <c r="N14" s="2">
+        <v>10943</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="2"/>
+        <v>11.493124343529015</v>
+      </c>
+      <c r="R14" s="2">
+        <v>18.381932973861598</v>
+      </c>
+      <c r="S14" s="2">
+        <v>8452</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1748619230787503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>12</v>
+      </c>
+      <c r="B15" s="10">
         <v>45253</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C15" s="8">
         <v>98.92</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D15" s="8">
         <v>95.83</v>
       </c>
-      <c r="E14" s="2">
-        <v>100</v>
-      </c>
-      <c r="F14" s="2">
-        <v>100</v>
-      </c>
-      <c r="G14" s="2">
-        <v>58.607282161712597</v>
-      </c>
-      <c r="H14" s="2">
-        <v>9160</v>
-      </c>
-      <c r="I14" s="2">
+      <c r="E15" s="8">
+        <v>100</v>
+      </c>
+      <c r="F15" s="8">
+        <v>100</v>
+      </c>
+      <c r="G15" s="6">
         <f t="shared" si="0"/>
         <v>6.3981749084839086</v>
       </c>
-      <c r="J14" s="2">
-        <v>100</v>
-      </c>
-      <c r="K14" s="2">
-        <v>100</v>
-      </c>
-      <c r="L14" s="2">
-        <v>359.86930632591202</v>
-      </c>
-      <c r="M14" s="2">
-        <v>11651</v>
-      </c>
-      <c r="N14">
+      <c r="H15" s="8">
+        <v>100</v>
+      </c>
+      <c r="I15" s="8">
+        <v>100</v>
+      </c>
+      <c r="J15" s="6">
         <f t="shared" si="1"/>
         <v>30.887417932015452</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3">
+      <c r="M15" s="2">
+        <v>359.86930632591202</v>
+      </c>
+      <c r="N15" s="2">
+        <v>11651</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="2"/>
+        <v>30.887417932015452</v>
+      </c>
+      <c r="R15" s="2">
+        <v>58.607282161712597</v>
+      </c>
+      <c r="S15" s="2">
+        <v>9160</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="3"/>
+        <v>6.3981749084839086</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>13</v>
+      </c>
+      <c r="B16" s="10">
         <v>45255</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C16" s="8">
         <v>97.38</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="8">
         <v>91.18</v>
       </c>
-      <c r="E15" s="2">
-        <v>100</v>
-      </c>
-      <c r="F15" s="2">
-        <v>100</v>
-      </c>
-      <c r="G15" s="2">
-        <v>31.2516734600067</v>
-      </c>
-      <c r="H15" s="2">
-        <v>9512</v>
-      </c>
-      <c r="I15" s="2">
+      <c r="E16" s="8">
+        <v>100</v>
+      </c>
+      <c r="F16" s="8">
+        <v>100</v>
+      </c>
+      <c r="G16" s="6">
         <f t="shared" si="0"/>
         <v>3.2854997329695861</v>
       </c>
-      <c r="J15" s="2">
-        <v>100</v>
-      </c>
-      <c r="K15" s="2">
-        <v>100</v>
-      </c>
-      <c r="L15" s="2">
-        <v>184.78754043579099</v>
-      </c>
-      <c r="M15" s="2">
-        <v>12003</v>
-      </c>
-      <c r="N15">
+      <c r="H16" s="8">
+        <v>100</v>
+      </c>
+      <c r="I16" s="8">
+        <v>100</v>
+      </c>
+      <c r="J16" s="6">
         <f t="shared" si="1"/>
         <v>15.395112924751395</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
+      <c r="M16" s="2">
+        <v>184.78754043579099</v>
+      </c>
+      <c r="N16" s="2">
+        <v>12003</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="2"/>
+        <v>15.395112924751395</v>
+      </c>
+      <c r="R16" s="2">
+        <v>31.2516734600067</v>
+      </c>
+      <c r="S16" s="2">
+        <v>9512</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="3"/>
+        <v>3.2854997329695861</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>14</v>
+      </c>
+      <c r="B17" s="10">
         <v>45262</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="8">
         <v>99.49</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="8">
         <v>97.14</v>
       </c>
-      <c r="E16" s="2">
-        <v>100</v>
-      </c>
-      <c r="F16" s="2">
-        <v>100</v>
-      </c>
-      <c r="G16" s="2">
-        <v>21.8337883949279</v>
-      </c>
-      <c r="H16" s="2">
-        <v>9804</v>
-      </c>
-      <c r="I16" s="2">
+      <c r="E17" s="8">
+        <v>100</v>
+      </c>
+      <c r="F17" s="8">
+        <v>100</v>
+      </c>
+      <c r="G17" s="6">
         <f t="shared" si="0"/>
         <v>2.2270286000538455</v>
       </c>
-      <c r="J16" s="2">
-        <v>100</v>
-      </c>
-      <c r="K16" s="2">
-        <v>100</v>
-      </c>
-      <c r="L16" s="2">
-        <v>136.205902814865</v>
-      </c>
-      <c r="M16" s="2">
-        <v>12295</v>
-      </c>
-      <c r="N16">
+      <c r="H17" s="8">
+        <v>100</v>
+      </c>
+      <c r="I17" s="8">
+        <v>100</v>
+      </c>
+      <c r="J17" s="6">
         <f t="shared" si="1"/>
         <v>11.078153949968685</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3">
+      <c r="M17" s="2">
+        <v>136.205902814865</v>
+      </c>
+      <c r="N17" s="2">
+        <v>12295</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="2"/>
+        <v>11.078153949968685</v>
+      </c>
+      <c r="R17" s="2">
+        <v>21.8337883949279</v>
+      </c>
+      <c r="S17" s="2">
+        <v>9804</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" si="3"/>
+        <v>2.2270286000538455</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>15</v>
+      </c>
+      <c r="B18" s="10">
         <v>45268</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="8">
         <v>99.45</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="8">
         <v>96.77</v>
       </c>
-      <c r="E17" s="2">
-        <v>100</v>
-      </c>
-      <c r="F17" s="2">
-        <v>100</v>
-      </c>
-      <c r="G17" s="2">
-        <v>32.015193700790398</v>
-      </c>
-      <c r="H17" s="2">
-        <v>10191</v>
-      </c>
-      <c r="I17" s="2">
+      <c r="E18" s="8">
+        <v>100</v>
+      </c>
+      <c r="F18" s="8">
+        <v>100</v>
+      </c>
+      <c r="G18" s="6">
         <f t="shared" si="0"/>
         <v>3.1415164067108625</v>
       </c>
-      <c r="J17" s="2">
-        <v>100</v>
-      </c>
-      <c r="K17" s="2">
-        <v>100</v>
-      </c>
-      <c r="L17" s="2">
-        <v>207.48235726356501</v>
-      </c>
-      <c r="M17" s="2">
-        <v>12682</v>
-      </c>
-      <c r="N17">
+      <c r="H18" s="8">
+        <v>100</v>
+      </c>
+      <c r="I18" s="8">
+        <v>100</v>
+      </c>
+      <c r="J18" s="6">
         <f t="shared" si="1"/>
         <v>16.360381427500787</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>19</v>
-      </c>
-      <c r="B18" s="3">
+      <c r="M18" s="2">
+        <v>207.48235726356501</v>
+      </c>
+      <c r="N18" s="2">
+        <v>12682</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="2"/>
+        <v>16.360381427500787</v>
+      </c>
+      <c r="R18" s="2">
+        <v>32.015193700790398</v>
+      </c>
+      <c r="S18" s="2">
+        <v>10191</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="3"/>
+        <v>3.1415164067108625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>16</v>
+      </c>
+      <c r="B19" s="10">
         <v>45269</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="8">
         <v>98.97</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="8">
         <v>95.59</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="8">
         <v>98.97</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="8">
         <v>95.59</v>
       </c>
-      <c r="G18" s="2">
-        <v>81.1793630123138</v>
-      </c>
-      <c r="H18" s="2">
-        <v>11113</v>
-      </c>
-      <c r="I18" s="2">
+      <c r="G19" s="6">
         <f t="shared" si="0"/>
         <v>7.3049008379657874</v>
       </c>
-      <c r="J18" s="2">
+      <c r="H19" s="8">
         <v>98.97</v>
       </c>
-      <c r="K18" s="2">
+      <c r="I19" s="8">
         <v>95.59</v>
       </c>
-      <c r="L18" s="2">
-        <v>370.983638763427</v>
-      </c>
-      <c r="M18" s="2">
-        <v>13515</v>
-      </c>
-      <c r="N18">
+      <c r="J19" s="6">
         <f t="shared" si="1"/>
         <v>27.44976979381628</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>20</v>
-      </c>
-      <c r="B19" s="3">
+      <c r="M19" s="2">
+        <v>370.983638763427</v>
+      </c>
+      <c r="N19" s="2">
+        <v>13515</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="2"/>
+        <v>27.44976979381628</v>
+      </c>
+      <c r="R19" s="2">
+        <v>81.1793630123138</v>
+      </c>
+      <c r="S19" s="2">
+        <v>11113</v>
+      </c>
+      <c r="T19" s="2">
+        <f t="shared" si="3"/>
+        <v>7.3049008379657874</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>17</v>
+      </c>
+      <c r="B20" s="11">
         <v>45270</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C20" s="8">
         <v>98.89</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="8">
         <v>95.71</v>
       </c>
-      <c r="E19" s="2">
-        <v>100</v>
-      </c>
-      <c r="F19" s="2">
-        <v>100</v>
-      </c>
-      <c r="G19" s="2">
-        <v>287.19313001632599</v>
-      </c>
-      <c r="H19" s="2">
-        <v>13306</v>
-      </c>
-      <c r="I19" s="2">
+      <c r="E20" s="8">
+        <v>100</v>
+      </c>
+      <c r="F20" s="8">
+        <v>100</v>
+      </c>
+      <c r="G20" s="6">
         <f t="shared" si="0"/>
         <v>21.583731400595671</v>
       </c>
-      <c r="J19" s="2">
-        <v>100</v>
-      </c>
-      <c r="K19" s="2">
-        <v>100</v>
-      </c>
-      <c r="L19" s="2">
-        <v>870.55976033210698</v>
-      </c>
-      <c r="M19" s="2">
-        <v>14953</v>
-      </c>
-      <c r="N19">
+      <c r="H20" s="8">
+        <v>100</v>
+      </c>
+      <c r="I20" s="8">
+        <v>100</v>
+      </c>
+      <c r="J20" s="6">
         <f t="shared" si="1"/>
         <v>58.219739204982744</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C20" s="2">
-        <f t="shared" ref="C20:H20" si="2">AVERAGE(C3:C19)</f>
+      <c r="M20" s="2">
+        <v>870.55976033210698</v>
+      </c>
+      <c r="N20" s="2">
+        <v>14953</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="2"/>
+        <v>58.219739204982744</v>
+      </c>
+      <c r="R20" s="2">
+        <v>287.19313001632599</v>
+      </c>
+      <c r="S20" s="2">
+        <v>13306</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" si="3"/>
+        <v>21.583731400595671</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17">
+        <f t="shared" ref="C21:F21" si="4">AVERAGE(C4:C20)</f>
         <v>97.904705882352943</v>
       </c>
-      <c r="D20" s="2">
-        <f t="shared" si="2"/>
+      <c r="D21" s="17">
+        <f t="shared" si="4"/>
         <v>92.157647058823542</v>
       </c>
-      <c r="E20" s="2">
-        <f t="shared" si="2"/>
+      <c r="E21" s="18">
+        <f t="shared" si="4"/>
         <v>99.145882352941172</v>
       </c>
-      <c r="F20" s="2">
-        <f t="shared" si="2"/>
+      <c r="F21" s="18">
+        <f t="shared" si="4"/>
         <v>96.791764705882343</v>
       </c>
-      <c r="G20" s="2">
-        <f t="shared" si="2"/>
-        <v>74.7236133743734</v>
-      </c>
-      <c r="H20" s="2">
-        <f t="shared" si="2"/>
-        <v>7771.588235294118</v>
-      </c>
-      <c r="I20" s="2">
+      <c r="G21" s="18">
         <f t="shared" si="0"/>
         <v>9.6149732991541406</v>
       </c>
-      <c r="J20" s="2">
-        <f t="shared" ref="J20:N20" si="3">AVERAGE(J3:J19)</f>
+      <c r="H21" s="18">
+        <f>AVERAGE(H4:H20)</f>
         <v>99.332941176470598</v>
       </c>
-      <c r="K20" s="2">
-        <f t="shared" si="3"/>
+      <c r="I21" s="18">
+        <f>AVERAGE(I4:I20)</f>
         <v>97.389999999999986</v>
       </c>
-      <c r="L20" s="2">
-        <f t="shared" si="3"/>
-        <v>436.23579028073436</v>
-      </c>
-      <c r="M20" s="2">
-        <f t="shared" si="3"/>
-        <v>10016.176470588236</v>
-      </c>
-      <c r="N20">
+      <c r="J21" s="18">
         <f t="shared" si="1"/>
         <v>43.553125442798319</v>
       </c>
-      <c r="O20" s="2">
-        <f>N20/I20</f>
+      <c r="M21" s="2">
+        <f t="shared" ref="K21:N21" si="5">AVERAGE(M4:M20)</f>
+        <v>436.23579028073436</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="5"/>
+        <v>10016.176470588236</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="2"/>
+        <v>43.553125442798319</v>
+      </c>
+      <c r="P21" s="2">
+        <f>O21/T21</f>
         <v>4.5297188133252355</v>
       </c>
+      <c r="R21" s="2">
+        <f>SUM(R4:R20)</f>
+        <v>1270.3014273643478</v>
+      </c>
+      <c r="S21" s="2">
+        <f>SUM(S4:S20)</f>
+        <v>132117</v>
+      </c>
+      <c r="T21" s="2">
+        <f>(R21/S21) * 1000</f>
+        <v>9.6149732991541406</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T22" s="2"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T23" s="2"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T24" s="2"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T25" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="12">
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G21" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>